<commit_message>
Ajout section IA avec 7 exercices pratiques: decouverte, amelioration texte, resumer, decision, prompting, limites, quotidien
</commit_message>
<xml_diff>
--- a/Excel/Exercice 1.xlsx
+++ b/Excel/Exercice 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eb92272b50bc787c/Documents/Formation365/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{04821479-9A92-4A24-938D-6581DCC5ADE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95A4AABD-97BC-466B-8E2E-45F61E5E13E2}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{04821479-9A92-4A24-938D-6581DCC5ADE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{13AE2D36-C844-48AE-B2E4-DCE9C15A1A07}"/>
   <bookViews>
-    <workbookView xWindow="492" yWindow="2688" windowWidth="17280" windowHeight="8880" xr2:uid="{985234DA-4007-48EC-88AF-5BA3708F5F0C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{985234DA-4007-48EC-88AF-5BA3708F5F0C}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -97,7 +97,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="dd/mm/yy;@"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -149,7 +149,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -159,7 +159,7 @@
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="171" formatCode="dd/mm/yy;@"/>
+      <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
     </dxf>
     <dxf>
       <font>
@@ -191,6 +191,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -533,7 +537,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>